<commit_message>
Added Timeline entities and views
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="TT" sheetId="1" r:id="rId1"/>
+    <sheet name="Order" sheetId="2" r:id="rId2"/>
+    <sheet name="TimeLine" sheetId="4" r:id="rId3"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="162">
   <si>
     <t>Важность</t>
   </si>
@@ -459,12 +460,84 @@
   <si>
     <t>List&lt;Employee&gt;.Where(x =&gt; x.Position.Contains("Машинист"))</t>
   </si>
+  <si>
+    <t>make bool values PZO and highAsh</t>
+  </si>
+  <si>
+    <t>refactoring and cleaning</t>
+  </si>
+  <si>
+    <t>create timeline and works</t>
+  </si>
+  <si>
+    <t>Adding/delete works for every machines via context menu on timeline</t>
+  </si>
+  <si>
+    <t>1 shift: 8:00 - 19:59</t>
+  </si>
+  <si>
+    <t>2 shift: 20:00 - 7:59</t>
+  </si>
+  <si>
+    <t>WORKS</t>
+  </si>
+  <si>
+    <t>Strat Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Technical operations</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Crushing burner</t>
+  </si>
+  <si>
+    <t>Loading of coal into vehicles</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>ash</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>wet</t>
+  </si>
+  <si>
+    <t>trapeze</t>
+  </si>
+  <si>
+    <t>rectangle</t>
+  </si>
+  <si>
+    <t>Coal preparation</t>
+  </si>
+  <si>
+    <t>count wagons</t>
+  </si>
+  <si>
+    <t>text-align at timeline table head and right some witdh for all cells</t>
+  </si>
+  <si>
+    <t>adding works to timeline</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,8 +578,41 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +636,40 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -982,11 +1122,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1052,10 +1194,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="1" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2096,7 +2252,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,15 +3325,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding works in time line added styles for different types of works
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="171">
   <si>
     <t>Важность</t>
   </si>
@@ -531,6 +531,33 @@
   </si>
   <si>
     <t>adding works to timeline</t>
+  </si>
+  <si>
+    <t>show start time and end time when click to work for editing</t>
+  </si>
+  <si>
+    <t>create styles for different types of works</t>
+  </si>
+  <si>
+    <t>show works on the timeline as need show style</t>
+  </si>
+  <si>
+    <t>create different styles for simple buttons and in tables</t>
+  </si>
+  <si>
+    <t>make to work show on timeline as at work time settings</t>
+  </si>
+  <si>
+    <t>create input-pattern and check for validation for values when creating work and order</t>
+  </si>
+  <si>
+    <t>input double nubmers with dot and ,</t>
+  </si>
+  <si>
+    <t>All cells some witdh</t>
+  </si>
+  <si>
+    <t>hide non-use fields when adding work depending on the type of work</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1155,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1182,6 +1209,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1194,18 +1233,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -2263,32 +2291,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -3364,7 +3392,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="49" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3374,24 +3402,24 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52" t="s">
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="54" t="s">
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="50" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3401,13 +3429,13 @@
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56" t="s">
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3437,13 +3465,13 @@
       </c>
     </row>
     <row r="25" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="58" t="s">
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="54" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3485,10 +3513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,28 +3525,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="57" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="58" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="57" t="s">
         <v>140</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="57" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="57" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="57" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring Staff, employeeManager, addid StaffAddDTO
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="183">
   <si>
     <t>Важность</t>
   </si>
@@ -558,6 +558,42 @@
   </si>
   <si>
     <t>hide non-use fields when adding work depending on the type of work</t>
+  </si>
+  <si>
+    <t>Iqueryable</t>
+  </si>
+  <si>
+    <t>async… await</t>
+  </si>
+  <si>
+    <t>viewModels</t>
+  </si>
+  <si>
+    <t>data transfer object</t>
+  </si>
+  <si>
+    <t>start-trime != end-time</t>
+  </si>
+  <si>
+    <t>precondition-postcondition</t>
+  </si>
+  <si>
+    <t>end-start</t>
+  </si>
+  <si>
+    <t>refactoring</t>
+  </si>
+  <si>
+    <t>dbaccess</t>
+  </si>
+  <si>
+    <t>validations</t>
+  </si>
+  <si>
+    <t>dto</t>
+  </si>
+  <si>
+    <t>viewmodels</t>
   </si>
 </sst>
 </file>
@@ -2280,7 +2316,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,10 +3549,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3574,24 +3610,80 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
order shift navigation repair and fixes
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,17 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="201">
   <si>
     <t>Важность</t>
   </si>
@@ -612,6 +607,42 @@
   </si>
   <si>
     <t>All async return Task</t>
+  </si>
+  <si>
+    <t>not delete from DB but add bool field IsDelete</t>
+  </si>
+  <si>
+    <t>lacale of time needs to repair</t>
+  </si>
+  <si>
+    <t>Допускается сделать ручное обновление страницы. Под вопросом: допускается сделать добавление работ не через контекстное меню, а просто через дополнительную панель.</t>
+  </si>
+  <si>
+    <t>error of non-close sesssion</t>
+  </si>
+  <si>
+    <t>error of non-contains in getById</t>
+  </si>
+  <si>
+    <t>error of show work, which was been delete on timeline</t>
+  </si>
+  <si>
+    <t>hide non-use fields when adding new work depending on the type of work</t>
+  </si>
+  <si>
+    <t>need to adding field of needs fields in class of type of work</t>
+  </si>
+  <si>
+    <t>repair DB</t>
+  </si>
+  <si>
+    <t>show old valid data when trying put invalid data in form and save</t>
+  </si>
+  <si>
+    <t>error of non-writable WEGTH on work of COAL PREPARATION</t>
+  </si>
+  <si>
+    <t>show works inline when their times is not crossing</t>
   </si>
 </sst>
 </file>
@@ -1275,6 +1306,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1287,7 +1319,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -2334,7 +2365,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,32 +2376,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="60" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="1:6" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2405,7 +2436,9 @@
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3567,10 +3600,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,7 +3611,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>138</v>
       </c>
@@ -3586,57 +3619,100 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="58" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="58" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="59" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="O7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L8" s="59" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L9" s="59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="L11" s="59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L12" s="59" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="59" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="63" t="s">
+      <c r="L13" s="59" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L14" s="59" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="59" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3661,7 +3737,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="59" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3712,7 +3788,7 @@
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="59" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3722,7 +3798,7 @@
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="59" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding backend for MachineryTable and TypesTable, need to make views
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="211">
   <si>
     <t>Важность</t>
   </si>
@@ -643,6 +643,36 @@
   </si>
   <si>
     <t>show works inline when their times is not crossing</t>
+  </si>
+  <si>
+    <t>Тип техники</t>
+  </si>
+  <si>
+    <t>Электрический</t>
+  </si>
+  <si>
+    <t>Автовскрыша</t>
+  </si>
+  <si>
+    <t>Дизельный</t>
+  </si>
+  <si>
+    <t>Ручной</t>
+  </si>
+  <si>
+    <t>Постообработка ошибки postcondition</t>
+  </si>
+  <si>
+    <t>need to make views</t>
+  </si>
+  <si>
+    <t>adding backend for machineryTable and adding</t>
+  </si>
+  <si>
+    <t>need to make backend for MachineryTypes table and adding</t>
+  </si>
+  <si>
+    <t>make views</t>
   </si>
 </sst>
 </file>
@@ -724,7 +754,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,6 +809,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,7 +1276,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1319,6 +1355,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -2365,7 +2403,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,10 +2527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AM69"/>
+  <dimension ref="A1:AM69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,7 +2543,21 @@
     <col min="15" max="15" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
       <c r="K2" s="4" t="s">
         <v>119</v>
       </c>
@@ -2513,7 +2565,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
       <c r="C3" s="12" t="s">
         <v>16</v>
       </c>
@@ -2584,7 +2642,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2659,7 +2723,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>18</v>
       </c>
@@ -2683,7 +2747,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2707,7 +2771,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
       <c r="D7" s="14"/>
       <c r="E7" s="8" t="s">
@@ -2729,7 +2793,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="D8" s="15"/>
       <c r="E8" s="11" t="s">
@@ -2751,7 +2815,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="D9" s="14"/>
       <c r="E9" s="8"/>
@@ -2774,7 +2838,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
       <c r="D10" s="14"/>
       <c r="E10" s="8"/>
@@ -2792,7 +2856,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C11" s="12" t="s">
         <v>25</v>
       </c>
@@ -2805,7 +2869,7 @@
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C12" s="9" t="s">
         <v>26</v>
       </c>
@@ -2818,7 +2882,7 @@
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>27</v>
       </c>
@@ -2831,7 +2895,7 @@
       </c>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="14"/>
       <c r="E14" s="8" t="s">
@@ -2842,7 +2906,7 @@
       </c>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="14"/>
       <c r="E15" s="8" t="s">
@@ -2853,7 +2917,7 @@
       </c>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="15"/>
       <c r="E16" s="11" t="s">
@@ -3603,7 +3667,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,37 +3775,57 @@
         <v>200</v>
       </c>
     </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L15" s="65" t="s">
+        <v>206</v>
+      </c>
+    </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L19" s="64" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L20" s="64" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L21" s="64"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="64" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="59" t="s">
+      <c r="L23" s="64" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="65" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
         <v>171</v>
       </c>
@@ -3749,7 +3833,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>172</v>
       </c>
@@ -3757,22 +3841,22 @@
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="57" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>176</v>
       </c>

</xml_diff>

<commit_message>
hide button find on the order
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -754,7 +754,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,12 +809,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1276,7 +1270,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1355,8 +1349,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -3667,7 +3659,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3776,7 +3768,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L15" s="65" t="s">
+      <c r="L15" s="58" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3789,7 +3781,7 @@
       <c r="A19" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="L19" s="64" t="s">
+      <c r="L19" s="57" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3797,7 +3789,7 @@
       <c r="A20" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="L20" s="64" t="s">
+      <c r="L20" s="57" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3805,10 +3797,9 @@
       <c r="A21" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="L21" s="64"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L22" s="64" t="s">
+      <c r="L22" s="57" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3816,12 +3807,12 @@
       <c r="A23" t="s">
         <v>170</v>
       </c>
-      <c r="L23" s="64" t="s">
+      <c r="L23" s="57" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="58" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding solve of conflict while changing type of machineries
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="231">
   <si>
     <t>Важность</t>
   </si>
@@ -700,6 +700,39 @@
   </si>
   <si>
     <t>Убрать радиобатоны</t>
+  </si>
+  <si>
+    <t>Появление и исчезновение полей без обновления страницы</t>
+  </si>
+  <si>
+    <t>Добавить категории должностей</t>
+  </si>
+  <si>
+    <t>Ошибка связана с неправильным рассчётом сдвига</t>
+  </si>
+  <si>
+    <t>Ошибка при добавлении работы в ночную смены, которая затрагивает время после полуночи</t>
+  </si>
+  <si>
+    <t>Change type of machinery</t>
+  </si>
+  <si>
+    <t>Solve the conflict on works</t>
+  </si>
+  <si>
+    <t>All data copying to new machines</t>
+  </si>
+  <si>
+    <t>Change all works in order</t>
+  </si>
+  <si>
+    <t>Group by order works which depending by changhing machineries</t>
+  </si>
+  <si>
+    <t>Сделать специальную viewModel класс копию класса Order, чтобы в нём не содержалось никаких удалённых оборудований и работ</t>
+  </si>
+  <si>
+    <t>Использовать этот класс везде, где только можно</t>
   </si>
 </sst>
 </file>
@@ -3683,10 +3716,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3804,7 +3837,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>162</v>
       </c>
@@ -3812,7 +3845,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>169</v>
       </c>
@@ -3820,17 +3853,23 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L22" s="57" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>170</v>
       </c>
@@ -3838,12 +3877,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q25" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
         <v>179</v>
       </c>
@@ -3857,7 +3891,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
         <v>171</v>
       </c>
@@ -3874,7 +3908,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>172</v>
       </c>
@@ -3891,7 +3925,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
         <v>173</v>
       </c>
@@ -3901,8 +3935,11 @@
       <c r="M29" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>174</v>
       </c>
@@ -3912,40 +3949,69 @@
       <c r="M30" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="57" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="57" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="59" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="57" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="59" t="s">
         <v>184</v>
+      </c>
+      <c r="L37" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try fluent validation to MVC in Positions Add action
</commit_message>
<xml_diff>
--- a/WebApplication3/2_5237915331338439750.xlsx
+++ b/WebApplication3/2_5237915331338439750.xlsx
@@ -708,12 +708,6 @@
     <t>Добавить категории должностей</t>
   </si>
   <si>
-    <t>Ошибка связана с неправильным рассчётом сдвига</t>
-  </si>
-  <si>
-    <t>Ошибка при добавлении работы в ночную смены, которая затрагивает время после полуночи</t>
-  </si>
-  <si>
     <t>Change type of machinery</t>
   </si>
   <si>
@@ -735,17 +729,23 @@
     <t>Использовать этот класс везде, где только можно</t>
   </si>
   <si>
-    <t>Передача массива в качестве параметров в котнроллер из представления</t>
-  </si>
-  <si>
-    <t>Ошибка при прохождении работы через полночь во второй смене</t>
+    <t>try to fluent validation to position add</t>
+  </si>
+  <si>
+    <t>add fluent validation to all project</t>
+  </si>
+  <si>
+    <t>decomposition</t>
+  </si>
+  <si>
+    <t>restructured project files to different folders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,14 +817,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1344,7 +1336,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1423,7 +1415,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -3731,10 +3722,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,7 +3733,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>138</v>
       </c>
@@ -3750,7 +3741,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>139</v>
       </c>
@@ -3758,18 +3749,15 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>140</v>
       </c>
       <c r="L3" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="U3" s="64" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>165</v>
       </c>
@@ -3777,7 +3765,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>160</v>
       </c>
@@ -3785,7 +3773,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
         <v>161</v>
       </c>
@@ -3793,7 +3781,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L7" s="59" t="s">
         <v>192</v>
       </c>
@@ -3801,17 +3789,17 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L8" s="59" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L9" s="59" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
         <v>163</v>
       </c>
@@ -3819,7 +3807,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
         <v>164</v>
       </c>
@@ -3827,38 +3815,35 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L12" s="59" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
         <v>167</v>
       </c>
       <c r="L13" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="T13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L14" s="59" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L15" s="58" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>162</v>
       </c>
@@ -3866,7 +3851,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>169</v>
       </c>
@@ -3874,31 +3859,25 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="T21" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L22" s="57" t="s">
         <v>209</v>
       </c>
-      <c r="T22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
         <v>170</v>
       </c>
       <c r="L23" s="57" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
         <v>179</v>
       </c>
@@ -3908,11 +3887,11 @@
       <c r="M26" t="s">
         <v>211</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26" s="58" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
         <v>171</v>
       </c>
@@ -3929,7 +3908,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>172</v>
       </c>
@@ -3946,7 +3925,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
         <v>173</v>
       </c>
@@ -3960,7 +3939,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>174</v>
       </c>
@@ -3974,65 +3953,110 @@
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q31" s="57" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>176</v>
       </c>
-      <c r="L32" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L32" s="57" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="L33" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L33" s="57" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="L34" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="L35" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L35" s="57" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="L36" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L36" s="57" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="L37" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L38" t="s">
-        <v>227</v>
+      <c r="L37" s="58" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L38" s="58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="33"/>
+      <c r="T41" s="33"/>
+      <c r="U41" s="33"/>
+      <c r="V41" s="33"/>
+      <c r="W41" s="33"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>